<commit_message>
hello made a change in commit + modified gitignore
</commit_message>
<xml_diff>
--- a/my.xlsx
+++ b/my.xlsx
@@ -16,9 +16,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>sdfgfdfv</t>
+  </si>
+  <si>
+    <t>dfghj</t>
+  </si>
+  <si>
+    <t>qsdfbn</t>
+  </si>
+  <si>
+    <t>asdfg</t>
+  </si>
+  <si>
+    <t>WDFGH</t>
+  </si>
+  <si>
+    <t>dfghjk</t>
+  </si>
+  <si>
+    <t>ghjk</t>
+  </si>
+  <si>
+    <t>sdfjkl</t>
+  </si>
+  <si>
+    <t>dfghjkl</t>
   </si>
 </sst>
 </file>
@@ -357,15 +381,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>